<commit_message>
update bug & delete old report
</commit_message>
<xml_diff>
--- a/PHPService/template2024_sample.xlsx
+++ b/PHPService/template2024_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tina.xue\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74AFF927-216F-4C8E-A2B8-487A2279CEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2C2831-EC30-4FBC-BEA5-B77DCEB29F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{58BF3F46-769F-7C44-81AF-97AE6FEE40FD}"/>
   </bookViews>
@@ -1332,7 +1332,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.4"/>
@@ -1556,7 +1556,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.4"/>
@@ -1599,21 +1599,21 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="15" t="e">
-        <f>Report!#REF!</f>
-        <v>#REF!</v>
+      <c r="A3" s="15">
+        <f>Report!$N4</f>
+        <v>0</v>
       </c>
       <c r="B3" s="12">
-        <f>IF(ISNUMBER(MATCH(LEFT(Report!#REF!,2),ref!$D$8:$D$113,0)),LEFT(Report!#REF!,2),0)</f>
+        <f>IF(ISNUMBER(MATCH(LEFT(Report!$E4,2),ref!$D$8:$D$113,0)),LEFT(Report!$E4,2),0)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="e">
-        <f>Report!#REF!</f>
-        <v>#REF!</v>
+      <c r="C3" s="12">
+        <f>Report!$G4</f>
+        <v>0</v>
       </c>
       <c r="D3" s="16" t="e">
-        <f>IF(ISNUMBER(MATCH($C3,ref!I33:I35,0)),WORKDAY($A3,VLOOKUP(C:C,ref!$I$32:$J$34,2,0),ref!$L$2:$L$6),WORKDAY($A3,IF(ISNUMBER(MATCH($B3,ref!$D$8:$D$113,0)),VLOOKUP(TAT原則!B:B,ref!$D$8:$F$113,3,0)),ref!C2:C6))</f>
-        <v>#REF!</v>
+        <f>IF(ISNUMBER(MATCH($C3,ref!I33:I35,0)),WORKDAY($A3,VLOOKUP(C:C,ref!$I$32:$J$34,2,0),ref!$L$2:$L$6),WORKDAY($A3,IF(ISNUMBER(MATCH($B3,ref!$D$8:$D$113,0)),VLOOKUP(TAT原則!B:B,ref!$D$8:$F$113,3,0)),ref!$L$2:$L$6))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A911A9-1609-4B6A-99B7-2E4DFA8D91D3}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>